<commit_message>
Temp changed MAster KFP
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/KFP/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/KFP/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_Muitisite\Input_files\Master_executors\ECTEST\KFP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018434A4-6F76-4E09-96D6-6C496332B4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D039828B-A94B-4C0C-9798-DD5F3A6E530D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="569" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MasterExecutor!$A$1:$F$29</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -435,16 +434,7 @@
     <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal 5" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -789,8 +779,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -856,7 +846,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>10</v>
@@ -876,7 +866,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>10</v>
@@ -896,7 +886,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>10</v>
@@ -916,7 +906,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>10</v>
@@ -936,7 +926,7 @@
         <v>66</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>10</v>
@@ -956,7 +946,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>10</v>
@@ -976,7 +966,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>10</v>
@@ -996,7 +986,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>10</v>
@@ -1016,7 +1006,7 @@
         <v>14</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>10</v>
@@ -1036,7 +1026,7 @@
         <v>26</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>10</v>
@@ -1056,7 +1046,7 @@
         <v>28</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>10</v>
@@ -1076,7 +1066,7 @@
         <v>30</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>10</v>
@@ -1096,7 +1086,7 @@
         <v>31</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>10</v>
@@ -1136,7 +1126,7 @@
         <v>35</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>10</v>
@@ -1156,7 +1146,7 @@
         <v>37</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>10</v>
@@ -1216,7 +1206,7 @@
         <v>43</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>10</v>
@@ -1236,7 +1226,7 @@
         <v>45</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>10</v>
@@ -1256,7 +1246,7 @@
         <v>47</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>10</v>
@@ -1296,7 +1286,7 @@
         <v>51</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>10</v>
@@ -1356,7 +1346,7 @@
         <v>56</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>10</v>
@@ -1376,7 +1366,7 @@
         <v>58</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Enabling all working testcases ECTEST KFP
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/KFP/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/KFP/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_Muitisite\Input_files\Master_executors\ECTEST\KFP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D039828B-A94B-4C0C-9798-DD5F3A6E530D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A506883-65A6-41E6-9489-AEF28A46577A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="569" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -776,11 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -846,7 +845,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>10</v>
@@ -866,7 +865,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>10</v>
@@ -886,7 +885,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>10</v>
@@ -906,7 +905,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>10</v>
@@ -926,7 +925,7 @@
         <v>66</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>10</v>
@@ -946,7 +945,7 @@
         <v>13</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>10</v>
@@ -966,7 +965,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F9" s="13" t="s">
         <v>10</v>
@@ -986,7 +985,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F10" s="11" t="s">
         <v>10</v>
@@ -1006,7 +1005,7 @@
         <v>14</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>10</v>
@@ -1026,7 +1025,7 @@
         <v>26</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>10</v>
@@ -1046,7 +1045,7 @@
         <v>28</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>10</v>
@@ -1066,7 +1065,7 @@
         <v>30</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F14" s="13" t="s">
         <v>10</v>
@@ -1086,13 +1085,13 @@
         <v>31</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="3" customFormat="1" hidden="1">
+    <row r="16" spans="1:6" s="3" customFormat="1">
       <c r="A16" s="11" t="s">
         <v>6</v>
       </c>
@@ -1126,7 +1125,7 @@
         <v>35</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>10</v>
@@ -1146,13 +1145,13 @@
         <v>37</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1">
+    <row r="19" spans="1:6">
       <c r="A19" s="11" t="s">
         <v>6</v>
       </c>
@@ -1172,7 +1171,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1">
+    <row r="20" spans="1:6">
       <c r="A20" s="11" t="s">
         <v>6</v>
       </c>
@@ -1206,7 +1205,7 @@
         <v>43</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>10</v>
@@ -1226,7 +1225,7 @@
         <v>45</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>10</v>
@@ -1246,13 +1245,13 @@
         <v>47</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" hidden="1">
+    <row r="24" spans="1:6">
       <c r="A24" s="11" t="s">
         <v>6</v>
       </c>
@@ -1286,13 +1285,13 @@
         <v>51</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" hidden="1">
+    <row r="26" spans="1:6" s="3" customFormat="1">
       <c r="A26" s="11" t="s">
         <v>6</v>
       </c>
@@ -1312,7 +1311,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="4" customFormat="1" hidden="1">
+    <row r="27" spans="1:6" s="4" customFormat="1">
       <c r="A27" s="11" t="s">
         <v>6</v>
       </c>
@@ -1346,7 +1345,7 @@
         <v>56</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>10</v>
@@ -1366,20 +1365,14 @@
         <v>58</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F29" s="11" t="s">
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F29" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F29" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Enabling all testcases KFP
</commit_message>
<xml_diff>
--- a/Input_files/Master_executors/ECTEST/KFP/MasterExecutor_Sanity.xlsx
+++ b/Input_files/Master_executors/ECTEST/KFP/MasterExecutor_Sanity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_Muitisite\Input_files\Master_executors\ECTEST\KFP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27D1FBE6-F7E8-4F49-B566-A079493554AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{272873CF-5C53-415C-BC4B-905AEE58E12F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="569" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -773,7 +773,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -839,7 +839,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>10</v>
@@ -859,7 +859,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>10</v>
@@ -879,7 +879,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>10</v>
@@ -899,7 +899,7 @@
         <v>11</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>10</v>
@@ -919,7 +919,7 @@
         <v>13</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F7" s="11" t="s">
         <v>10</v>
@@ -939,7 +939,7 @@
         <v>21</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>10</v>
@@ -959,7 +959,7 @@
         <v>23</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>10</v>
@@ -979,7 +979,7 @@
         <v>14</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F10" s="13" t="s">
         <v>10</v>
@@ -999,7 +999,7 @@
         <v>26</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>10</v>
@@ -1019,7 +1019,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>10</v>
@@ -1039,7 +1039,7 @@
         <v>30</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>10</v>
@@ -1059,7 +1059,7 @@
         <v>31</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>10</v>
@@ -1079,7 +1079,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>10</v>
@@ -1099,7 +1099,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>10</v>
@@ -1119,7 +1119,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>10</v>
@@ -1139,7 +1139,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>10</v>
@@ -1179,7 +1179,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>10</v>
@@ -1199,7 +1199,7 @@
         <v>64</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F21" s="11" t="s">
         <v>10</v>
@@ -1219,7 +1219,7 @@
         <v>45</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F22" s="11" t="s">
         <v>10</v>
@@ -1239,7 +1239,7 @@
         <v>47</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>10</v>
@@ -1259,7 +1259,7 @@
         <v>49</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F24" s="11" t="s">
         <v>10</v>
@@ -1279,7 +1279,7 @@
         <v>51</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F25" s="11" t="s">
         <v>10</v>
@@ -1319,7 +1319,7 @@
         <v>54</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>10</v>
@@ -1339,7 +1339,7 @@
         <v>56</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>10</v>

</xml_diff>